<commit_message>
mudança coluna - descartar - teste Edu
</commit_message>
<xml_diff>
--- a/cutover/Cutover_Execution_plan_Rev01.xlsx
+++ b/cutover/Cutover_Execution_plan_Rev01.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\carlos.franceschi\Documents\Reserva\Syngenta\PMO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eduardo_spirito\Documents\Syngenta ASM\compart\syngenta-appmap\cutover\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="349">
   <si>
     <t>ID</t>
   </si>
@@ -1448,10 +1448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F126"/>
+  <dimension ref="A1:G126"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1463,7 +1463,7 @@
     <col min="6" max="6" width="12.7109375" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -1482,8 +1482,11 @@
       <c r="F1" s="9" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>17</v>
       </c>
@@ -1500,7 +1503,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>21</v>
       </c>
@@ -1517,7 +1520,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>23</v>
       </c>
@@ -1534,7 +1537,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>28</v>
       </c>
@@ -1551,7 +1554,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>32</v>
       </c>
@@ -1568,7 +1571,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>36</v>
       </c>
@@ -1585,7 +1588,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>40</v>
       </c>
@@ -1602,7 +1605,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>44</v>
       </c>
@@ -1619,7 +1622,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>48</v>
       </c>
@@ -1636,7 +1639,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>49</v>
       </c>
@@ -1653,7 +1656,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>53</v>
       </c>
@@ -1670,7 +1673,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>54</v>
       </c>
@@ -1687,7 +1690,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>56</v>
       </c>
@@ -1704,7 +1707,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>60</v>
       </c>
@@ -1721,7 +1724,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>64</v>
       </c>

</xml_diff>

<commit_message>
tradução feedback, novas linhas para o cutover
</commit_message>
<xml_diff>
--- a/cutover/Cutover_Execution_plan_Rev01.xlsx
+++ b/cutover/Cutover_Execution_plan_Rev01.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\carlos.franceschi\Documents\Reserva\Syngenta\PMO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T966104\Documents\repos\docs\syngenta-appmap\cutover\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="364">
   <si>
     <t>ID</t>
   </si>
@@ -1071,6 +1071,51 @@
   </si>
   <si>
     <t>155;163</t>
+  </si>
+  <si>
+    <t>Dynasys</t>
+  </si>
+  <si>
+    <t>Master Data Uploads</t>
+  </si>
+  <si>
+    <t>Server upgrade 2003 to 2008</t>
+  </si>
+  <si>
+    <t>2 day</t>
+  </si>
+  <si>
+    <t>TMS - Kewill</t>
+  </si>
+  <si>
+    <t>E-Kanban</t>
+  </si>
+  <si>
+    <t>Stop application</t>
+  </si>
+  <si>
+    <t>Change the web.config to SAP FOU</t>
+  </si>
+  <si>
+    <t>Start application</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Specify the TMS Kewill WebService URL Endpoint on SAP Foundation server </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Specify the SAP Foundation URL on TMS Kewill server to POST inbound shipments </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PricingSpot </t>
+  </si>
+  <si>
+    <t>In the server friawotcssisp1 Stop windows service WSDespesasNutradePRO</t>
+  </si>
+  <si>
+    <t>In the server friawotcssisp1 search for http://syngenta1.pro.intra/pricingspot in the IIS and stop it</t>
+  </si>
+  <si>
+    <t>In the FRIAPSQLGL02\INSGLOB02 instance make the backup for the database PricingSPoT</t>
   </si>
 </sst>
 </file>
@@ -1114,7 +1159,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -1143,6 +1188,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1448,16 +1496,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F126"/>
+  <dimension ref="A1:F140"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="B141" sqref="B141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="4"/>
-    <col min="2" max="2" width="68.85546875" customWidth="1"/>
+    <col min="2" max="2" width="93.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.140625" style="4"/>
     <col min="4" max="5" width="21" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.7109375" style="4" bestFit="1" customWidth="1"/>
@@ -3644,6 +3692,127 @@
         <v>348</v>
       </c>
     </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A127" s="4">
+        <v>171</v>
+      </c>
+      <c r="B127" s="7" t="s">
+        <v>349</v>
+      </c>
+      <c r="C127" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A128" s="4">
+        <v>172</v>
+      </c>
+      <c r="B128" s="11" t="s">
+        <v>350</v>
+      </c>
+      <c r="C128" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" s="4">
+        <v>173</v>
+      </c>
+      <c r="B129" s="11" t="s">
+        <v>351</v>
+      </c>
+      <c r="C129" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" s="4">
+        <v>174</v>
+      </c>
+      <c r="B130" s="7" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" s="4">
+        <v>175</v>
+      </c>
+      <c r="B131" s="11" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132" s="4">
+        <v>176</v>
+      </c>
+      <c r="B132" s="11" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133" s="4">
+        <v>177</v>
+      </c>
+      <c r="B133" s="7" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134" s="4">
+        <v>178</v>
+      </c>
+      <c r="B134" s="3" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135" s="4">
+        <v>179</v>
+      </c>
+      <c r="B135" s="3" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136" s="4">
+        <v>180</v>
+      </c>
+      <c r="B136" s="3" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137" s="4">
+        <v>181</v>
+      </c>
+      <c r="B137" s="7" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138" s="4">
+        <v>182</v>
+      </c>
+      <c r="B138" s="3" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139" s="4">
+        <v>183</v>
+      </c>
+      <c r="B139" s="3" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140" s="4">
+        <v>184</v>
+      </c>
+      <c r="B140" s="3" t="s">
+        <v>362</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>